<commit_message>
figures of lcs patterns
</commit_message>
<xml_diff>
--- a/simplefly/bigtest/results_2.xlsx
+++ b/simplefly/bigtest/results_2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellahuang/Documents/Boulder/spring '20/independent study/fireflies/simplefly/bigtest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B33C9854-E6FB-E343-9463-D65B5C740F50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB2FD2D-83BF-0D4E-ACC2-FD86A94925A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15440"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="27640" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -337,8 +337,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -473,8 +473,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,6 +659,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -815,9 +828,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1172,11 +1188,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1186,10 +1202,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
@@ -1198,10 +1214,10 @@
       <c r="D1">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J1" t="s">
@@ -1212,10 +1228,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
@@ -1224,10 +1240,10 @@
       <c r="D2">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J2" t="s">
@@ -1238,10 +1254,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
@@ -1250,7 +1266,7 @@
       <c r="D3">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I3" t="s">
@@ -1334,7 +1350,7 @@
       <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
@@ -1360,13 +1376,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D7">
@@ -1416,7 +1432,7 @@
       <c r="I8" t="s">
         <v>71</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K8">
@@ -1433,7 +1449,7 @@
       <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D9">

</xml_diff>